<commit_message>
Upload Diagram Metadata Reports for Rel 5.3
</commit_message>
<xml_diff>
--- a/Documents/Diagram Metadata Reports/BRIDG5.3Beta-20190205/BRIDG5.3Beta-20190204-Activities.xlsx
+++ b/Documents/Diagram Metadata Reports/BRIDG5.3Beta-20190205/BRIDG5.3Beta-20190204-Activities.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wverhoef\Documents\BRIDG\BRIDG R5.3\EA Diagram Report Development\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Julie Evans\Documents\GitHub\bridg-model\Documents\Diagram Metadata Reports\BRIDG5.3Beta-20190205\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3675DF05-B4DB-4B5E-B018-D6EB3662684C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="90" windowWidth="23895" windowHeight="14535"/>
+    <workbookView xWindow="8420" yWindow="155" windowWidth="8035" windowHeight="10200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Diagram_Metadata_Report" sheetId="1" r:id="rId1"/>
@@ -178,7 +179,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -345,6 +346,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -380,6 +398,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -555,33 +590,33 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="16.26953125" style="2" customWidth="1"/>
     <col min="2" max="2" width="21" style="2" customWidth="1"/>
-    <col min="3" max="5" width="9.140625" style="2"/>
-    <col min="6" max="6" width="122.7109375" style="3" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="2"/>
+    <col min="3" max="5" width="9.1328125" style="2"/>
+    <col min="6" max="6" width="122.7265625" style="3" customWidth="1"/>
+    <col min="7" max="16384" width="9.1328125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="21" x14ac:dyDescent="0.75">
       <c r="A1" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="18.5" x14ac:dyDescent="0.75">
       <c r="A2" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A3" s="5" t="s">
         <v>0</v>
       </c>
@@ -601,7 +636,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="165" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="162.25" x14ac:dyDescent="0.75">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
@@ -612,7 +647,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="240" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="206.5" x14ac:dyDescent="0.75">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
@@ -623,7 +658,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="375" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="368.75" x14ac:dyDescent="0.75">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
@@ -634,7 +669,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="225" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="221.25" x14ac:dyDescent="0.75">
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
@@ -645,7 +680,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="165" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="147.5" x14ac:dyDescent="0.75">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
@@ -656,7 +691,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="180" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="147.5" x14ac:dyDescent="0.75">
       <c r="A9" s="2" t="s">
         <v>6</v>
       </c>
@@ -667,7 +702,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="375" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="339.25" x14ac:dyDescent="0.75">
       <c r="A10" s="2" t="s">
         <v>6</v>
       </c>

</xml_diff>